<commit_message>
[Sandra] LLM evaluation of different question types, compared to GPT-4
</commit_message>
<xml_diff>
--- a/project/evaluation/llm_evaluation/question_types/testset_different_question_types.xlsx
+++ b/project/evaluation/llm_evaluation/question_types/testset_different_question_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandrafriebolin/Desktop/WS23-24/nlpt_group/project/evaluation/llm_evaluation/question_types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E347F063-CB0F-174D-B937-F2435A0FE829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9107C2-146E-E349-B0F8-E493D1CC8EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{11B363AB-6081-C140-A8D6-8FFAD50DF30B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t>Question</t>
   </si>
@@ -54,10 +54,6 @@
   </si>
   <si>
     <t>GPT-4 without Context</t>
-  </si>
-  <si>
-    <t>Based on the provided information, the association between intelligence and lifespan appears to be largely genetic. The analysis of data from three genetically informative samples, including twin studies from the US, Sweden, and Denmark, supports a genetic relationship between intelligence and lifespan. The meta-analysis of these studies showed a small positive phenotypic correlation between intelligence and lifespan, with an observed correlation coefficient of .12. Importantly, the additive genetic covariance model indicated that the genetic contribution to the covariance between intelligence and lifespan was significantly high, with the combined sample showing a 95% genetic contribution. This high percentage of genetic contribution was consistent across the individual studies from the US (84%), Sweden (86%), and Denmark (85%).
-These findings suggest that the relationship between intelligence and lifespan is not solely due to environmental factors like socioeconomic status or health behaviors, but rather, there is a substantial genetic basis to this association. This has significant implications for public health and research into the genetics of intelligence, lifespan, and health inequalities, highlighting the importance of genetic factors in understanding the link between intelligence and lifespan.</t>
   </si>
   <si>
     <t>The association between intelligence and lifespan involves a complex interplay of genetic, environmental, and lifestyle factors. Here's an overview of how these elements can interact:
@@ -79,15 +75,6 @@
   </si>
   <si>
     <t>Is regular breakfast consumption associated with increased IQ in kindergarten children?</t>
-  </si>
-  <si>
-    <t>GPT-4 with Context
-Prompt: You are a medical QA-assistant. Answer the following question only based on the provided information:
-Question:
-Information:</t>
-  </si>
-  <si>
-    <t>Based on the provided information, regular breakfast consumption is indeed associated with increased IQ in kindergarten children. This conclusion comes from a cross-sectional study conducted with a sample of 1269 children aged 6 years from Jintan, China. The study found that children who regularly consumed breakfast on a near-daily basis had significantly higher scores in full scale, verbal, and performance IQ tests compared to children who sometimes ate breakfast. This association remained significant for verbal IQ (VIQ) and full IQ (FIQ) even after adjusting for several socioeconomic and parental psychosocial variables. These findings suggest that the benefits of regular breakfast consumption on cognition may stem from both nutritional and social factors, emphasizing the importance of encouraging regular breakfast consumption among young children.</t>
   </si>
   <si>
     <t>Regular breakfast consumption has been associated with various benefits in children, including improved cognitive function, better academic performance, and overall healthier dietary habits. However, the specific link between regular breakfast consumption and an increase in IQ among kindergarten children requires examination of scientific research to determine if there's a direct correlation.
@@ -107,15 +94,6 @@
   </si>
   <si>
     <t>Explore the relationship between genetic factors and intelligence variations in monozygotic twins.</t>
-  </si>
-  <si>
-    <t>The relationship between genetic factors and intelligence variations in monozygotic (MZ) twins, as illuminated by the provided information, presents a complex interaction between genetics, environmental factors, and individual differences in intelligence and school performance. MZ twins, despite having identical genotypes, exhibit variations in school performance, which is considered a stable and heritable psychological characteristic. This variation suggests that factors beyond genetics contribute to differences in intelligence and educational outcomes.
-The findings from the study of 2,768 MZ twin pairs highlight several key points:
-1. **Stability of Differences**: MZ differences in school performance are moderately stable from age 12 through 16, indicating that the variations observed are not merely transient but persist through critical stages of educational development. This stability points to the enduring influence of non-genetic factors on educational outcomes.
-2. **Correlation Across Variables**: The positive correlation between MZ differences in school performance and differences across 16 learning-related variables—including measures of intelligence, personality, and school attitudes—suggests a multifaceted relationship between these factors. The twin scoring higher in one aspect also tends to score higher in others, indicating that the variations in performance are not isolated but part of a broader pattern of individual differences.
-3. **Systematic Influence of Nonshared Environment**: Contrary to the idiosyncratic and chance-driven effects previously assumed, the findings suggest that nonshared environmental factors systematically affect school performance. These factors account for 22% of the variance in MZ differences in school performance at age 16, emphasizing the significant role of individual experiences and environments in shaping educational outcomes even among genetically identical individuals.
-4. **Search for Nonshared Environmental Factors**: The study underscores the need to identify the specific nonshared environmental factors that contribute to these systematic and stable differences in school performance among MZ twins. Understanding these factors could inform educational strategies and interventions tailored to individual needs.
-In summary, the relationship between genetic factors and intelligence variations in MZ twins is influenced by a combination of genetic predispositions and nonshared environmental factors. While genetic factors provide a baseline, the variations in intelligence and school performance among MZ twins are significantly shaped by individual experiences, attitudes, and environmental contexts. This highlights the importance of considering both genetic and environmental factors in educational planning and individualized learning approaches.</t>
   </si>
   <si>
     <t>The relationship between genetic factors and intelligence variations in monozygotic (identical) twins provides a fascinating insight into the nature vs. nurture debate, especially as it pertains to intelligence. Monozygotic twins are genetically identical, having originated from the same fertilized egg that split into two embryos. This unique situation allows researchers to study the effects of different environments on individuals with the same genetic makeup.
@@ -143,11 +121,6 @@
     <t>Is there a correlation between working memory and fluid intelligence across children with developmental disorders?</t>
   </si>
   <si>
-    <t>Based on the provided information, there is an indication of a correlation between working memory (WM) and fluid intelligence across children with developmental disorders, as evidenced by the study's evaluation of children with Developmental Language Disorder (DLD), high-functioning children with Autism Spectrum Disorder (ASD), and children with Down syndrome (DS). The study utilized different measures of phonological working memory, visual-spatial working memory, and fluid intelligence, measured with Raven Progressive Matrices, to investigate these relationships.
-The analysis revealed significant differences among the three groups in both individual functions and their correlations. Specifically, the DLD and high-functioning ASD groups showed overlapping performances across all phonological and visual-spatial working memory measures, with the exception of the Backward Digit Recall task. This suggests a common pattern of working memory capacity and possibly its relationship to fluid intelligence in these groups. In contrast, the DS group exhibited unique working memory patterns, differing significantly from the DLD and high-functioning ASD groups, indicating a different correlation pattern between working memory and fluid intelligence for children with DS.
-The study's findings highlight the complex relationship between working memory and fluid intelligence across different developmental disorders, suggesting that while there may be a general correlation between these cognitive functions, the nature and extent of the correlation can vary significantly among different groups of children with developmental disorders. The distinct working memory patterns observed, particularly in the DS group compared to the DLD and high-functioning ASD groups, underscore the necessity for further research to understand these relationships fully and to tailor support for learning and development accordingly.</t>
-  </si>
-  <si>
     <t>Yes, there is a significant correlation between working memory and fluid intelligence across children with developmental disorders, as well as typically developing children. Working memory is the capacity to hold and manipulate information in mind over short periods, while fluid intelligence refers to the ability to solve novel reasoning problems and adapt to new situations without relying on previously acquired knowledge.
 Research indicates that working memory capacities are closely linked to fluid intelligence across various populations. This relationship is evident in children with developmental disorders such as ADHD, autism spectrum disorders, dyslexia, and specific language impairment, among others. These disorders often involve deficits in working memory, which in turn can impact fluid intelligence and other cognitive abilities.
 For children with developmental disorders, difficulties in working memory can lead to challenges in learning, problem-solving, and academic achievement, given the role of working memory in supporting fluid intelligence. Interventions aimed at enhancing working memory skills can therefore be beneficial in improving not only working memory itself but also fluid intelligence and related cognitive functions.
@@ -182,22 +155,7 @@
     <t>Based on the discovery that mitochondrial dysfunction plays an important role in Alzheimer's disease, how could interventions aimed at improving mitochondrial function affect the treatment or management of Alzheimer's disease?</t>
   </si>
   <si>
-    <t>The Theory of Multiple Intelligences (MI), proposed by Howard Gardner, differentiates cognitive abilities by suggesting that intelligence is not a single, unified faculty but a collection of various cognitive capabilities. This theory contrasts with traditional views that measure intelligence through IQ tests, focusing on linguistic and mathematical abilities. Gardner's MI theory posits that individuals possess a range of intelligences, each representing different ways of processing information and solving problems.
-The article discusses MI theory's relevance and application in teacher education programs, emphasizing its comparison to learning styles theory. Unlike learning styles, which suggest that people have preferred ways of receiving and processing information, MI theory identifies distinct forms of intelligence, such as linguistic, logical-mathematical, spatial, musical, bodily-kinesthetic, interpersonal, intrapersonal, and naturalist intelligences. This broader conceptualization of intelligence underlines the importance of addressing diverse cognitive abilities within educational contexts.
-Furthermore, the article highlights the significance of incorporating Universal Design for Learning (UDL) and related frameworks into teacher education curricula. UDL is an educational framework that aims to improve and optimize teaching and learning for all people based on scientific insights into how humans learn. By acknowledging and leveraging the diverse intelligences identified by MI theory, educators can better tailor their teaching strategies to meet the varied learning needs of their students. This approach advocates for a more inclusive and effective educational environment that recognizes and values the multiple ways individuals understand and engage with the world.G6</t>
-  </si>
-  <si>
     <t>Should artificial intelligence surpass human intelligence in diagnostic accuracy, what ethical considerations would arise in relying on AI for making critical healthcare decisions?</t>
-  </si>
-  <si>
-    <t>The discovery that mitochondrial dysfunction, particularly deficits in energy homeostasis, plays a significant role in Alzheimer's disease (AD) suggests that interventions aimed at improving mitochondrial function could have a profound impact on the treatment and management of AD. The identified dysregulation in genes involved in mitochondrial energy (ATP) and oxidative phosphorylation in the frontal cortex, and mitochondrial cellular biosynthesis and mitochondrial ribosomes in the cerebellum, highlights the critical role of mitochondria in AD pathology.
-Interventions aimed at enhancing mitochondrial function could potentially address these dysregulations by:
-1. **Improving Energy Homeostasis**: Enhancing the efficiency of ATP production and oxidative phosphorylation could help restore energy balance in neuronal cells, which is crucial for maintaining cellular functions and survival. This could mitigate the energy deficit observed in AD, potentially slowing down the progression of neurodegeneration.
-2. **Reducing Oxidative Stress**: Dysfunctional mitochondria are a major source of reactive oxygen species (ROS), which contribute to oxidative stress and neuronal damage in AD. Interventions that improve mitochondrial function could reduce the production of ROS, thereby decreasing oxidative stress and its detrimental effects on brain cells.
-3. **Enhancing Mitochondrial Biogenesis and Maintenance**: Targeting pathways that promote mitochondrial biogenesis and maintenance could help compensate for the loss and dysfunction of mitochondria in AD. This could involve the activation of signaling pathways that promote the formation of new mitochondria and the repair of damaged ones.
-4. **Stabilizing Mitochondrial Dynamics**: Mitochondrial dynamics, including fusion and fission processes, are essential for maintaining mitochondrial function and integrity. Interventions that stabilize these dynamics could prevent or mitigate mitochondrial fragmentation, a feature observed in AD, thus preserving neuronal health and function.
-5. **Targeting Specific Dysregulated Genes**: The identification of specific dysregulated genes, such as ATP5L and ATP5H, offers the opportunity for targeted gene therapy. Restoring the expression or function of these genes could directly address the mitochondrial deficits observed in AD.
-In summary, interventions aimed at improving mitochondrial function could offer a multi-faceted approach to AD treatment by addressing the underlying energy deficits, reducing oxidative stress, and correcting specific mitochondrial dysfunctions. This could potentially slow disease progression, improve symptoms, or even provide a novel avenue for the prevention of AD. However, the translation of these interventions from theoretical or experimental models to clinical practice requires extensive research and clinical trials to assess their efficacy and safety in humans.</t>
   </si>
   <si>
     <t>The discovery that mitochondrial dysfunction plays an important role in Alzheimer's disease (AD) offers promising new avenues for the treatment and management of the condition. Mitochondria, often referred to as the powerhouses of the cell, are responsible for producing energy and regulating cellular metabolism. In the context of Alzheimer's disease, mitochondrial dysfunction can lead to decreased energy production, increased oxidative stress, and ultimately contribute to the neurodegenerative processes characteristic of AD.
@@ -248,15 +206,220 @@
   <si>
     <t>What are the key components of emotional intelligence as it relates to patient care in nursing?</t>
   </si>
+  <si>
+    <t>Does tick-borne encephalitis carry a high risk of incomplete recovery in children?</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+        No, the association between intelligence and lifespan is mostly due to environmental factors such as socioeconomic status and health behaviors. However, there are also some genetic components involved. The study found that the genetic contribution to the covariance between intelligence and lifespan was about 85% in the US study, 84% in the Swedish study, and 86% in the Danish study.&lt;/p&gt;
+&lt;p&gt;For more information, please refer to the following links:&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/26213105' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/26213105&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/28088056' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/28088056&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/26014827' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/26014827&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+        Yes, regular breakfast consumption is associated with increased IQ in kindergarten children. The study conducted in China found that children who regularly have breakfast on a neardaily basis had significantly higher full scale verbal and performance IQ test scores compared to those who sometimes have breakfast. The relationship persists for VIQ verbal IQ and FIQ full IQ even after adjusting for various sociodemographic and psychological factors.&lt;/p&gt;
+&lt;p&gt;For more information, please refer to the following links:&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/34204553' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/34204553&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/23395328' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/23395328&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+        Several studies have explored the relationship between genetic factors and intelligence variations in monozygotic twins. One study found that there is no genetic correlation between general factors of intelligence and personality despite both being selected for in human evolution. Another study found that different indexes of visual search performance were moderately heritable and only a small proportion of the genetic variance in visual search was shared with genetic variance in intelligence.&lt;/p&gt;
+&lt;p&gt;For more information, please refer to the following links:&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/25991074' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/25991074&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/23358157' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/23358157&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/35044053' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/35044053&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/25056688' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/25056688&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+        Yes, according to the study, a large proportion of children experience an incomplete recovery after tick-borne encephalitis (TBE).
+        The most prevalent cognitive deficits in these children include problems in executive function and working memory.
+        However, the study also notes that many children recover well and return to their daily lives and previous activities.&lt;/p&gt;
+&lt;p&gt;For more information, please refer to the following links:&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/33889554' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/33889554&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/23452585' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/23452585&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/34827386' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/34827386&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/24534397' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/24534397&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Tick-borne encephalitis (TBE) is a viral infectious disease involving the central nervous system, transmitted by the bite of infected ticks. The disease can vary in severity from mild to severe, involving the meninges (meningitis), the brain (encephalitis), or the spinal cord and brain (meningoencephalitis).
+In children, as in adults, the risk of incomplete recovery after TBE can depend on several factors, including the severity of the initial illness, the specific virus subtype, and the timeliness and appropriateness of medical treatment. However, children often have a more favorable prognosis than adults. Severe outcomes and long-term neurological sequelae are less common in children, but they are not unheard of.
+Incomplete recovery may manifest as persistent headaches, muscle weakness, cognitive difficulties, or other neurological symptoms. The European subtype of TBE virus tends to be associated with a more severe course of illness and a higher risk of incomplete recovery compared to the Siberian and Far Eastern subtypes, although all can cause severe disease.
+Preventative measures, including vaccination in regions where TBE is endemic, wearing protective clothing, and using tick repellents, are crucial in reducing the risk of TBE. Early diagnosis and treatment are important to manage symptoms and potentially reduce the risk of long-term complications.
+For the most current and detailed information, consulting sources that specialize in infectious diseases or neurology, especially those focusing on pediatric populations, would be beneficial. Research and guidelines on TBE and its outcomes in children are continually evolving, so up-to-date information from health authorities or recent studies would provide the most accurate picture of risks and prognosis.</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;1. The relationship between fluid intelligence and working memory is of fundamental importance to understanding how capacity-limited structures such as working memory interact with inference abilities to determine intelligent behavior.
+        2. Recent evidence has suggested that the relationship between a fluid abilities test Ravens Progressive Matrices and working memory capacity WMC may be invariant across difficulty levels of the Ravens items.
+        3. The simulation results were confirmed by two studies that used a composite measure of WMC which yielded a higher correlation between WMC and Ravens than reported in previous studies.&lt;/p&gt;
+&lt;p&gt;For more information, please refer to the following links:&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/24711798' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/24711798&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/35370868' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/35370868&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/33826402' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/33826402&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/26718618' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/26718618&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+        The Theory of Multiple Intelligences (MI) posits that human intelligence is made up of various types of intelligences rather than just one general intelligence. These intelligences include verbal-linguistic, visual-spatial, interpersonal, intrapersonal, naturalistic, logical-mathematical, bodily-kinesthetic, and musical. Each person has a unique combination of these intelligences, and they differ in terms of their strengths and weaknesses.&lt;/p&gt;
+&lt;p&gt;For more information, please refer to the following links:&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/34041385' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/34041385&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/29342659' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/29342659&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/33252596' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/33252596&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+        Interventions aimed at improving mitochondrial function could potentially help manage Alzheimer's disease by reducing oxidative stress and promoting neurogenesis. Specifically, drugs that enhance mitochondrial biogenesis and reduce oxidative stress could be useful in treating Alzheimer's disease. Additionally, lifestyle interventions such as exercise and dietary changes could also improve mitochondrial function and potentially slow the progression of Alzheimer's disease.&lt;/p&gt;
+&lt;p&gt;For more information, please refer to the following links:&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/32443912' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/32443912&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/36618979' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/36618979&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/38137886' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/38137886&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/35037261' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/35037261&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+        If AI surpassed human intelligence in diagnostic accuracy, ethical considerations would arise in relying on AI for making critical healthcare decisions. These include issues of bias, accountability, and transparency. Additionally, there would be concerns about the potential loss of jobs for healthcare professionals and the impact on patient autonomy and informed consent. Therefore, it is important to strike a balance between utilizing AI's strengths and maintaining the integrity of human expertise in healthcare decision-making.&lt;/p&gt;
+&lt;p&gt;For more information, please refer to the following links:&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/36543108' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/36543108&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/38135293' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/38135293&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/38143615' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/38143615&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/38028967' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/38028967&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;1. Vocabulary
+        2. Fluid reasoning
+        3. Working memory
+        4. Processing speed&lt;/p&gt;
+&lt;p&gt;For more information, please refer to the following links:&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/24927516' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/24927516&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/35249585' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/35249585&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/25349093' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/25349093&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/32059087' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/32059087&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;
+        Emotional intelligence (EI) refers to the ability to recognize, understand, and manage one's own emotions and those of others. In nursing, EI plays a crucial role in improving patient care by facilitating effective communication, building trust, and promoting empathy. Key components of EI in nursing include self-awareness, self-regulation, empathy, and social skills.&lt;/p&gt;
+&lt;p&gt;For more information, please refer to the following links:&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/31497624' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/31497624&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/29135748' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/29135748&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/37074163' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/37074163&lt;/a&gt;&lt;/p&gt;
+&lt;p&gt;&lt;a href='https://pubmed.ncbi.nlm.nih.gov/37727434' target='_blank'&gt;https://pubmed.ncbi.nlm.nih.gov/37727434&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Emotional intelligence (EI) is crucial in nursing as it directly impacts patient care quality. The key components of emotional intelligence as it relates to patient care in nursing include:
+1. **Self-awareness**: Nurses need to understand their own emotions, strengths, weaknesses, and how their emotional state can affect their interactions with patients. This awareness helps in managing stress and maintaining a professional demeanor even in challenging situations.
+2. **Self-regulation**: This involves the ability to control or redirect disruptive emotions and impulses. For nurses, self-regulation is essential in managing emotional responses in a way that is appropriate to the professional environment, ensuring that personal feelings do not interfere with patient care.
+3. **Motivation**: A high level of motivation is necessary for nurses to provide high-quality care, overcome challenges, and engage in continuous learning and improvement. This component of emotional intelligence drives nurses to pursue goals with energy and persistence.
+4. **Empathy**: Empathy is the ability to understand and share the feelings of another. In nursing, it's crucial for creating a strong patient-nurse relationship. Empathy enables nurses to understand patients' perspectives and needs better, providing care that is more responsive and tailored to individual patients.
+5. **Social skills**: Good social skills allow nurses to communicate effectively, build relationships, work in teams, and manage conflicts. These skills are essential in a collaborative environment like healthcare, where nurses must interact with patients, families, and other healthcare professionals.
+Incorporating these components of emotional intelligence into patient care enables nurses to provide compassionate, empathetic, and effective care, contributing to better patient outcomes and satisfaction. Emotionally intelligent nurses are also better equipped to handle the stresses of their job, reducing burnout and improving overall job satisfaction.</t>
+  </si>
+  <si>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t>Wrong answer! Retrieved documents in fact find a correlation between intelligence and lifespan.</t>
+  </si>
+  <si>
+    <t>Preferred answer, more detailed, correctly refers to evidence for correlation.</t>
+  </si>
+  <si>
+    <t>Correct &amp; preferred answer. Gves correct facts from the study, thus justifying its decision.</t>
+  </si>
+  <si>
+    <t>Too general. Does not "know" of specific studies and thus cannot give expected answer.</t>
+  </si>
+  <si>
+    <t>Nice overview about what different studies found out. Together with linked papers, this is the preferred answer.</t>
+  </si>
+  <si>
+    <t>More detailed answer, but it is not possible to verify all the facts, therefore not trustworthy despite detailed explanation</t>
+  </si>
+  <si>
+    <t>Nice, compact answer with reference to specific study on this issue.</t>
+  </si>
+  <si>
+    <t>Gives too much information that was not asked for (like preventative measures). Can thus be overwhelming/not interessting when looking only for specific answer to question.</t>
+  </si>
+  <si>
+    <t>Answer correctly indicates the significant relationship between working memory (WMC) and fluid intelligence, proving ist decision by concrete evidence and reference to specific study results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too general. </t>
+  </si>
+  <si>
+    <t>Here, the more general answer is preferred as it better explains this theory.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This answer lists aspects but does not clarify </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>how</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the theory differentiates cognitive abilities</t>
+    </r>
+  </si>
+  <si>
+    <t>Nice compact answer with precise overview of two strategies.</t>
+  </si>
+  <si>
+    <t>Again more detailed and broad overview.</t>
+  </si>
+  <si>
+    <t>Too many points listed.</t>
+  </si>
+  <si>
+    <t>Shortly lists most important points to consider.</t>
+  </si>
+  <si>
+    <t>Very short answer, but correctly lists domains.</t>
+  </si>
+  <si>
+    <t>List again too long, can be onverwhelming.</t>
+  </si>
+  <si>
+    <t>Nice compact answer, listing key components.</t>
+  </si>
+  <si>
+    <t>Preferred answer because list is manageable.</t>
+  </si>
+  <si>
+    <t>Our system produces the preferred answer for 70% of the queries</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,16 +437,59 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC3A6F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8DCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE1FFF2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC1FFD7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5D00B6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -291,19 +497,132 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color auto="1"/>
+      </left>
+      <right style="mediumDashed">
+        <color auto="1"/>
+      </right>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -311,6 +630,20 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF5D00B6"/>
+      <color rgb="FFC1FFD7"/>
+      <color rgb="FFB5FFED"/>
+      <color rgb="FFE1FFF2"/>
+      <color rgb="FFD4F2FD"/>
+      <color rgb="FFD3FCF7"/>
+      <color rgb="FFE8DCFF"/>
+      <color rgb="FFC3A6F3"/>
+      <color rgb="FFD6FFF5"/>
+      <color rgb="FFB4EBFD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -639,206 +972,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF77C09D-ADD9-ED4D-AF66-AE74B629F22B}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.5" customWidth="1"/>
-    <col min="2" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="44.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="44.5" style="12" customWidth="1"/>
+    <col min="7" max="7" width="54.5" style="18" customWidth="1"/>
+    <col min="8" max="8" width="54.5" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="14" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="409.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>26213105</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>26213105</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
+      <c r="C3" s="1">
+        <v>23395328</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>23395328</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
+    <row r="4" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>29920866</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>14</v>
+      <c r="E4" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1">
+        <v>23452585</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>29920866</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="C6" s="1">
+        <v>35370868</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H6" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C7" s="1">
+        <v>35814048</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>35370868</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="s">
+    <row r="8" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>23</v>
+      <c r="C8" s="2">
+        <v>36618979</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="9" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6">
-        <v>35814048</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>26</v>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="11" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2">
-        <v>36618979</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>32</v>
+      <c r="E11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>33</v>
+    <row r="12" spans="1:8" s="25" customFormat="1" ht="364" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-    </row>
+    <row r="13" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A13:XFD13"/>
+    <mergeCell ref="A12:XFD12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>